<commit_message>
create and fill scaled dataset05 whole body cropping table (babb02.1 and babb03, whole body)
</commit_message>
<xml_diff>
--- a/dataset03-cropping-table-babb03.xlsx
+++ b/dataset03-cropping-table-babb03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\imageProcessTif\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dancer\Documents\imageProcessTif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6C2FD9-0602-4946-9D1F-651606F07AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C18467-A750-4667-AB7D-3D0888030D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{2D0EAEAB-47F1-498F-A59D-91F173EB47DA}"/>
+    <workbookView xWindow="28680" yWindow="2505" windowWidth="21840" windowHeight="13740" xr2:uid="{2D0EAEAB-47F1-498F-A59D-91F173EB47DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -678,37 +678,37 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="0.77734375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="4"/>
+    <col min="8" max="8" width="0.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" customWidth="1"/>
     <col min="16" max="16" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="0.77734375" customWidth="1"/>
+    <col min="17" max="17" width="0.7109375" customWidth="1"/>
     <col min="18" max="19" width="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="8" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" style="4" customWidth="1"/>
-    <col min="23" max="24" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -782,7 +782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -942,7 +942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>22</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>21</v>
       </c>

</xml_diff>